<commit_message>
Added more scenarios with data driven approach
</commit_message>
<xml_diff>
--- a/src/data/users.xlsx
+++ b/src/data/users.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kumar Freelancing\Poc-pageObjectModel-Framework\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1cfb4c1c5457b90f/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC85D323-2332-46C5-BDD8-C2DCE1DC2CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{5AC295A6-B9C9-43CD-8768-CA62281F0CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{626426F1-2557-48D4-8FE0-FF9351AD54A1}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FEB0A234-1382-48F5-B39C-61B209382999}"/>
   </bookViews>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>userNameFromExcel</t>
   </si>
@@ -47,7 +45,7 @@
     <t>student</t>
   </si>
   <si>
-    <t>kulkarni</t>
+    <t>Password123</t>
   </si>
 </sst>
 </file>
@@ -100,6 +98,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -419,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53111CA1-9DB8-48F7-8634-CB788D72BBC4}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -447,6 +449,22 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>